<commit_message>
Added UC:Edit Org, UC: Archive Shift
</commit_message>
<xml_diff>
--- a/UseCase/UseCaseDescriptions.xlsx
+++ b/UseCase/UseCaseDescriptions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
   <si>
     <t>Table 1</t>
   </si>
@@ -137,6 +137,82 @@
   <si>
     <t>1. System determines that a shift is duplicate, System prompts user that shift already exists  2. System determines that necessary fields have not been filled and does not have enough information to create the shift, System prompts the user to fill in necessary fields</t>
+  </si>
+  <si>
+    <t>Edit Organization</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>Admin will be able to edit details about the organization</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Organizations will be able to use the scheduler software after contacting and registering with an Admin.</t>
+  </si>
+  <si>
+    <t>Low - We don’t expect to edit details about an organization often</t>
+  </si>
+  <si>
+    <t>1. The user selects an existing organization</t>
+  </si>
+  <si>
+    <t>The user must be viewing a list of existing organizations</t>
+  </si>
+  <si>
+    <t>The new details of the organization will overwrite the existing ones.</t>
+  </si>
+  <si>
+    <t>1. System queries and displays a list of existing organizations with similar names +2. User selects existing organization +3. System displays organization details in a form +4. User selects and edits form details +5. System prompts user to confirm changes to the organization +6. System overwrites existing data with new changes</t>
+  </si>
+  <si>
+    <t>1. System determines that necessary fields have been left blank and prompts the user to fill in those fields +2. System determines that the changes will cause a conflict in the database and warns the user before discarding changes</t>
+  </si>
+  <si>
+    <t>Archive Shift</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>Old shifts will be archived for read only purposes</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Organizations will be able to see past shift data in order to better plan future shifts which will lead to better productivity and moral</t>
+  </si>
+  <si>
+    <t>Moderate - We expect shifts to be archived after each schedule expires</t>
+  </si>
+  <si>
+    <t>1. System determines that the current time is greater than the schedule expire time</t>
+  </si>
+  <si>
+    <t>Schedule must have been created and shifts must have been assigned</t>
+  </si>
+  <si>
+    <t>Shifts that belong to the old schedule are moved into an archive table</t>
+  </si>
+  <si>
+    <t>1. System determines that it is time to start the next schedule +2. System moves old shifts into archive</t>
+  </si>
+  <si>
+    <t>1. Admin manually archives shifts</t>
+  </si>
+  <si>
+    <t>1. System determines that there is not enough space to move shifts and warns the admin</t>
   </si>
 </sst>
 </file>
@@ -146,7 +222,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -158,13 +234,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,12 +266,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -202,9 +289,7 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
@@ -214,8 +299,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -224,7 +340,62 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -233,28 +404,28 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -262,12 +433,28 @@
       <left style="thin">
         <color indexed="11"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -279,41 +466,68 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -333,8 +547,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="fffefb66"/>
       <rgbColor rgb="ffdbdbdb"/>
@@ -354,10 +570,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -534,11 +750,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -547,27 +766,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -824,10 +1043,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1118,7 +1337,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1399,222 +1618,580 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:B27"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="111.727" style="1" customWidth="1"/>
-    <col min="3" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="111.672" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="A3" t="s" s="10">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" t="s" s="11">
         <v>2</v>
       </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="A4" t="s" s="12">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" t="s" s="13">
         <v>4</v>
       </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="6">
+      <c r="A5" t="s" s="12">
         <v>5</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="B5" t="s" s="13">
         <v>6</v>
       </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="A6" t="s" s="12">
         <v>7</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="B6" t="s" s="13">
         <v>8</v>
       </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" ht="32.05" customHeight="1">
-      <c r="A7" t="s" s="6">
+      <c r="A7" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="B7" t="s" s="7">
+      <c r="B7" t="s" s="13">
         <v>10</v>
       </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="6">
+      <c r="A8" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="B8" t="s" s="7">
+      <c r="B8" t="s" s="13">
         <v>12</v>
       </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="6">
+      <c r="A9" t="s" s="12">
         <v>13</v>
       </c>
-      <c r="B9" t="s" s="7">
+      <c r="B9" t="s" s="13">
         <v>14</v>
       </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="6">
+      <c r="A10" t="s" s="12">
         <v>15</v>
       </c>
-      <c r="B10" t="s" s="7">
+      <c r="B10" t="s" s="13">
         <v>16</v>
       </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" ht="56.05" customHeight="1">
-      <c r="A11" t="s" s="6">
+      <c r="A11" t="s" s="12">
         <v>17</v>
       </c>
-      <c r="B11" t="s" s="7">
+      <c r="B11" t="s" s="13">
         <v>18</v>
       </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" ht="68.05" customHeight="1">
-      <c r="A12" t="s" s="6">
+      <c r="A12" t="s" s="12">
         <v>19</v>
       </c>
-      <c r="B12" t="s" s="7">
+      <c r="B12" t="s" s="13">
         <v>20</v>
       </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="6">
+      <c r="A13" t="s" s="12">
         <v>21</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" ht="32.05" customHeight="1">
-      <c r="A14" t="s" s="6">
+      <c r="A14" t="s" s="12">
         <v>22</v>
       </c>
-      <c r="B14" t="s" s="7">
+      <c r="B14" t="s" s="13">
         <v>23</v>
       </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="10">
+      <c r="A16" t="s" s="16">
         <v>1</v>
       </c>
-      <c r="B16" t="s" s="11">
+      <c r="B16" t="s" s="17">
         <v>24</v>
       </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="6">
+      <c r="A17" t="s" s="12">
         <v>3</v>
       </c>
-      <c r="B17" t="s" s="7">
+      <c r="B17" t="s" s="13">
         <v>25</v>
       </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="6">
+      <c r="A18" t="s" s="12">
         <v>5</v>
       </c>
-      <c r="B18" t="s" s="7">
+      <c r="B18" t="s" s="13">
         <v>26</v>
       </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="6">
+      <c r="A19" t="s" s="12">
         <v>7</v>
       </c>
-      <c r="B19" t="s" s="7">
+      <c r="B19" t="s" s="13">
         <v>27</v>
       </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" ht="32.05" customHeight="1">
-      <c r="A20" t="s" s="6">
+      <c r="A20" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="B20" t="s" s="7">
+      <c r="B20" t="s" s="13">
         <v>28</v>
       </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="6">
+      <c r="A21" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="B21" t="s" s="7">
+      <c r="B21" t="s" s="13">
         <v>29</v>
       </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" ht="32.05" customHeight="1">
-      <c r="A22" t="s" s="6">
+      <c r="A22" t="s" s="12">
         <v>13</v>
       </c>
-      <c r="B22" t="s" s="7">
+      <c r="B22" t="s" s="13">
         <v>30</v>
       </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="6">
+      <c r="A23" t="s" s="12">
         <v>15</v>
       </c>
-      <c r="B23" t="s" s="7">
+      <c r="B23" t="s" s="13">
         <v>31</v>
       </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" ht="32.05" customHeight="1">
-      <c r="A24" t="s" s="6">
+      <c r="A24" t="s" s="12">
         <v>17</v>
       </c>
-      <c r="B24" t="s" s="7">
+      <c r="B24" t="s" s="13">
         <v>32</v>
       </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" ht="68.05" customHeight="1">
-      <c r="A25" t="s" s="6">
+      <c r="A25" t="s" s="12">
         <v>19</v>
       </c>
-      <c r="B25" t="s" s="7">
+      <c r="B25" t="s" s="13">
         <v>33</v>
       </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" ht="44.05" customHeight="1">
-      <c r="A26" t="s" s="6">
+      <c r="A26" t="s" s="12">
         <v>21</v>
       </c>
-      <c r="B26" t="s" s="7">
+      <c r="B26" t="s" s="13">
         <v>34</v>
       </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" ht="44.05" customHeight="1">
-      <c r="A27" t="s" s="6">
+      <c r="A27" t="s" s="12">
         <v>22</v>
       </c>
-      <c r="B27" t="s" s="7">
+      <c r="B27" t="s" s="13">
         <v>35</v>
       </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" ht="14.7" customHeight="1">
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" ht="22.6" customHeight="1">
+      <c r="A29" t="s" s="16">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s" s="17">
+        <v>36</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" ht="14.7" customHeight="1">
+      <c r="A30" t="s" s="12">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s" s="13">
+        <v>37</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" ht="14.7" customHeight="1">
+      <c r="A31" t="s" s="12">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s" s="13">
+        <v>38</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" ht="14.7" customHeight="1">
+      <c r="A32" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s" s="13">
+        <v>39</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" ht="26.7" customHeight="1">
+      <c r="A33" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s" s="13">
+        <v>40</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" ht="14.7" customHeight="1">
+      <c r="A34" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s" s="13">
+        <v>41</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" ht="14.7" customHeight="1">
+      <c r="A35" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s" s="13">
+        <v>42</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
+    </row>
+    <row r="36" ht="14.7" customHeight="1">
+      <c r="A36" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s" s="13">
+        <v>43</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
+    </row>
+    <row r="37" ht="14.7" customHeight="1">
+      <c r="A37" t="s" s="12">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s" s="13">
+        <v>44</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" ht="74.7" customHeight="1">
+      <c r="A38" t="s" s="12">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s" s="13">
+        <v>45</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
+    </row>
+    <row r="39" ht="14.7" customHeight="1">
+      <c r="A39" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9"/>
+    </row>
+    <row r="40" ht="26.7" customHeight="1">
+      <c r="A40" t="s" s="12">
+        <v>22</v>
+      </c>
+      <c r="B40" t="s" s="13">
+        <v>46</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="9"/>
+    </row>
+    <row r="41" ht="14.7" customHeight="1">
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9"/>
+    </row>
+    <row r="42" ht="21.95" customHeight="1">
+      <c r="A42" t="s" s="16">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s" s="17">
+        <v>47</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="9"/>
+    </row>
+    <row r="43" ht="14.7" customHeight="1">
+      <c r="A43" t="s" s="12">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s" s="13">
+        <v>48</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="9"/>
+    </row>
+    <row r="44" ht="14.7" customHeight="1">
+      <c r="A44" t="s" s="12">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s" s="13">
+        <v>49</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="9"/>
+    </row>
+    <row r="45" ht="14.7" customHeight="1">
+      <c r="A45" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s" s="13">
+        <v>50</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="9"/>
+    </row>
+    <row r="46" ht="26.7" customHeight="1">
+      <c r="A46" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s" s="13">
+        <v>51</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" ht="14.7" customHeight="1">
+      <c r="A47" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s" s="13">
+        <v>52</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" ht="14.7" customHeight="1">
+      <c r="A48" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="B48" t="s" s="13">
+        <v>53</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" ht="14.7" customHeight="1">
+      <c r="A49" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="B49" t="s" s="13">
+        <v>54</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" ht="14.7" customHeight="1">
+      <c r="A50" t="s" s="12">
+        <v>17</v>
+      </c>
+      <c r="B50" t="s" s="13">
+        <v>55</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="9"/>
+    </row>
+    <row r="51" ht="26.7" customHeight="1">
+      <c r="A51" t="s" s="12">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s" s="13">
+        <v>56</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="9"/>
+    </row>
+    <row r="52" ht="14.7" customHeight="1">
+      <c r="A52" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="9"/>
+    </row>
+    <row r="53" ht="14.7" customHeight="1">
+      <c r="A53" t="s" s="12">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s" s="13">
+        <v>58</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>